<commit_message>
Outputting CSV with all the relevant fields and their values, could also generate GRADE from the PERC in the future, should be trivial. Same for YOS_CODE.
Unsure about the importance of CRN, RSTS_CODE, RECTYPE, ROLL_DATE, GCHG_CODE, GCDG_DESC, GCMT_CODE, GCMT_DESC, OPPORTUNITY, RESIT_FLAG, RELEASE_IND, COHORT.
</commit_message>
<xml_diff>
--- a/ProgrammeData.xlsx
+++ b/ProgrammeData.xlsx
@@ -550,7 +550,7 @@
     <t xml:space="preserve">F2P1-CSA_group_2</t>
   </si>
   <si>
-    <t xml:space="preserve">BSc Computer Science (Cyber Secuirty)</t>
+    <t xml:space="preserve">BSc Computer Science (Cyber Security)</t>
   </si>
   <si>
     <t xml:space="preserve">F2C3-CCS</t>
@@ -2053,11 +2053,11 @@
   </sheetPr>
   <dimension ref="A1:I1193"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A765" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D784" activeCellId="0" sqref="D784"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H129" activeCellId="0" sqref="H129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.77"/>

</xml_diff>